<commit_message>
Added Delegates to Delegate-Front
</commit_message>
<xml_diff>
--- a/Cards/DelegateData/Delegate-Front.xlsx
+++ b/Cards/DelegateData/Delegate-Front.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tech\Github Repos\TEAM-TEAM-TraitorCards\Cards\PeopleData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tech\Github Repos\TEAM-TEAM-TraitorCards\Cards\DelegateData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3100A75D-DB24-440B-A886-33A678B7ADA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEC89362-BDD7-44D3-96D7-AC1B87B070C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1E0E38A4-A720-4B05-94AE-F55473173966}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="32">
   <si>
     <t>Name</t>
   </si>
@@ -48,6 +48,90 @@
   </si>
   <si>
     <t>EffectText</t>
+  </si>
+  <si>
+    <t>@ComboIcon</t>
+  </si>
+  <si>
+    <t>ComboText</t>
+  </si>
+  <si>
+    <t>ComboPrefix</t>
+  </si>
+  <si>
+    <t>Poisoner</t>
+  </si>
+  <si>
+    <t>Assassin</t>
+  </si>
+  <si>
+    <t>Doctor</t>
+  </si>
+  <si>
+    <t>Knight</t>
+  </si>
+  <si>
+    <t>Bodydouble</t>
+  </si>
+  <si>
+    <t>Saboteur</t>
+  </si>
+  <si>
+    <t>Legion</t>
+  </si>
+  <si>
+    <t>Poisoner.ai</t>
+  </si>
+  <si>
+    <t>Assassin.ai</t>
+  </si>
+  <si>
+    <t>Doctor.ai</t>
+  </si>
+  <si>
+    <t>Knight.ai</t>
+  </si>
+  <si>
+    <t>Bodydouble.ai</t>
+  </si>
+  <si>
+    <t>Saboteur.ai</t>
+  </si>
+  <si>
+    <t>Legion.ai</t>
+  </si>
+  <si>
+    <t>Damage.ai</t>
+  </si>
+  <si>
+    <t>Protection.ai</t>
+  </si>
+  <si>
+    <t>x1</t>
+  </si>
+  <si>
+    <t>x2</t>
+  </si>
+  <si>
+    <t>x3</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>with Poisoneer</t>
+  </si>
+  <si>
+    <t>x2 with Poisoneer</t>
+  </si>
+  <si>
+    <t>x2 with Trap</t>
+  </si>
+  <si>
+    <t>with Assassin</t>
+  </si>
+  <si>
+    <t>x2 with Assassin</t>
   </si>
 </sst>
 </file>
@@ -97,7 +181,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -105,8 +189,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -442,23 +532,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81838662-B590-45E0-82FF-5E356D98D8D1}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.7109375" customWidth="1"/>
-    <col min="2" max="2" width="30.85546875" customWidth="1"/>
-    <col min="3" max="3" width="32.85546875" customWidth="1"/>
-    <col min="4" max="4" width="66.28515625" customWidth="1"/>
-    <col min="5" max="5" width="26.28515625" customWidth="1"/>
-    <col min="6" max="6" width="25.85546875" customWidth="1"/>
+    <col min="1" max="1" width="27" customWidth="1"/>
+    <col min="2" max="2" width="25.85546875" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="30.5703125" customWidth="1"/>
+    <col min="7" max="7" width="46.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -471,28 +562,171 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Corrected spelling of Poisoner
</commit_message>
<xml_diff>
--- a/Cards/DelegateData/Delegate-Front.xlsx
+++ b/Cards/DelegateData/Delegate-Front.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tech\Github Repos\TEAM-TEAM-TraitorCards\Cards\DelegateData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEC89362-BDD7-44D3-96D7-AC1B87B070C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68FC115A-19CE-443D-AFD4-03FB63EEEC8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1E0E38A4-A720-4B05-94AE-F55473173966}"/>
   </bookViews>
@@ -119,12 +119,6 @@
     <t>+</t>
   </si>
   <si>
-    <t>with Poisoneer</t>
-  </si>
-  <si>
-    <t>x2 with Poisoneer</t>
-  </si>
-  <si>
     <t>x2 with Trap</t>
   </si>
   <si>
@@ -132,6 +126,12 @@
   </si>
   <si>
     <t>x2 with Assassin</t>
+  </si>
+  <si>
+    <t>with Poisoner</t>
+  </si>
+  <si>
+    <t>x2 with Poisoner</t>
   </si>
 </sst>
 </file>
@@ -535,7 +535,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -609,7 +609,7 @@
         <v>21</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -632,7 +632,7 @@
         <v>22</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -655,7 +655,7 @@
         <v>22</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -678,7 +678,7 @@
         <v>22</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -701,7 +701,7 @@
         <v>21</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -724,7 +724,7 @@
         <v>22</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated combos on Delegate cards
</commit_message>
<xml_diff>
--- a/Cards/DelegateData/Delegate-Front.xlsx
+++ b/Cards/DelegateData/Delegate-Front.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tech\Github Repos\TEAM-TEAM-TraitorCards\Cards\DelegateData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68FC115A-19CE-443D-AFD4-03FB63EEEC8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40CCD7AE-4330-4F5D-A0C9-7780163930DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1E0E38A4-A720-4B05-94AE-F55473173966}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t>Name</t>
   </si>
@@ -44,21 +44,12 @@
     <t>@Image</t>
   </si>
   <si>
-    <t>@EffectIcon</t>
-  </si>
-  <si>
     <t>EffectText</t>
   </si>
   <si>
-    <t>@ComboIcon</t>
-  </si>
-  <si>
     <t>ComboText</t>
   </si>
   <si>
-    <t>ComboPrefix</t>
-  </si>
-  <si>
     <t>Poisoner</t>
   </si>
   <si>
@@ -101,37 +92,34 @@
     <t>Legion.ai</t>
   </si>
   <si>
-    <t>Damage.ai</t>
-  </si>
-  <si>
-    <t>Protection.ai</t>
-  </si>
-  <si>
-    <t>x1</t>
-  </si>
-  <si>
-    <t>x2</t>
-  </si>
-  <si>
-    <t>x3</t>
-  </si>
-  <si>
-    <t>+</t>
-  </si>
-  <si>
-    <t>x2 with Trap</t>
-  </si>
-  <si>
-    <t>with Assassin</t>
-  </si>
-  <si>
-    <t>x2 with Assassin</t>
-  </si>
-  <si>
-    <t>with Poisoner</t>
-  </si>
-  <si>
-    <t>x2 with Poisoner</t>
+    <t>-1 HP</t>
+  </si>
+  <si>
+    <t>-2 HP</t>
+  </si>
+  <si>
+    <t>+1 HP</t>
+  </si>
+  <si>
+    <t>+2 HP</t>
+  </si>
+  <si>
+    <t>-3 HP</t>
+  </si>
+  <si>
+    <t>+3 HP</t>
+  </si>
+  <si>
+    <t>Destroys one Poisoner</t>
+  </si>
+  <si>
+    <t>Destroys one Saboteur</t>
+  </si>
+  <si>
+    <t>Destroys one Assassin</t>
+  </si>
+  <si>
+    <t>1 extra damage with a Poisoner</t>
   </si>
 </sst>
 </file>
@@ -532,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81838662-B590-45E0-82FF-5E356D98D8D1}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -543,188 +531,117 @@
     <col min="1" max="1" width="27" customWidth="1"/>
     <col min="2" max="2" width="25.85546875" customWidth="1"/>
     <col min="3" max="3" width="22.7109375" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" customWidth="1"/>
-    <col min="6" max="6" width="30.5703125" customWidth="1"/>
-    <col min="7" max="7" width="46.140625" customWidth="1"/>
+    <col min="4" max="4" width="38.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="B4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D6" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-    </row>
-    <row r="3" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" s="5" t="s">
+      <c r="D8" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>